<commit_message>
Work Schedule for KISH-34
Work Schedule for KISH-34
</commit_message>
<xml_diff>
--- a/Civilworks cost/Work Schedule/Kishoregonj Packages/finalestimate_kishoregonjprotectivework/Flood Fuse -14_12.10.2020/Flood Fuse -14_12.10.2020/Pac-34/Estimate Segrigation.xlsx
+++ b/Civilworks cost/Work Schedule/Kishoregonj Packages/finalestimate_kishoregonjprotectivework/Flood Fuse -14_12.10.2020/Flood Fuse -14_12.10.2020/Pac-34/Estimate Segrigation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="76">
   <si>
     <t>Mobilization and Site Preparation</t>
   </si>
@@ -214,9 +214,6 @@
   </si>
   <si>
     <t>Type_A_78M_M25925_TO_M26003</t>
-  </si>
-  <si>
-    <t>Geo Bag Placing(125 Kg)</t>
   </si>
   <si>
     <t>Close Turfing</t>
@@ -259,7 +256,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -394,7 +391,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -436,7 +433,6 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -771,25 +767,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V67"/>
+  <dimension ref="A1:V71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="D13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19:H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" customWidth="1"/>
-    <col min="9" max="15" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" customWidth="1"/>
+    <col min="6" max="6" width="20.88671875" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" customWidth="1"/>
+    <col min="9" max="15" width="15.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="43.2">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -799,43 +795,43 @@
       <c r="C1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="I1" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="J1" s="30" t="s">
+      <c r="J1" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="K1" s="30" t="s">
+      <c r="K1" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="L1" s="30" t="s">
+      <c r="L1" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="M1" s="30" t="s">
+      <c r="M1" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="N1" s="30" t="s">
+      <c r="N1" s="29" t="s">
         <v>64</v>
       </c>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -854,26 +850,26 @@
       <c r="H2" s="2">
         <v>110</v>
       </c>
-      <c r="I2" s="33">
+      <c r="I2" s="32">
         <v>72</v>
       </c>
-      <c r="J2" s="33">
+      <c r="J2" s="32">
         <v>133</v>
       </c>
-      <c r="K2" s="33">
+      <c r="K2" s="32">
         <v>105</v>
       </c>
-      <c r="L2" s="33">
-        <v>100</v>
-      </c>
-      <c r="M2" s="33">
+      <c r="L2" s="32">
+        <v>100</v>
+      </c>
+      <c r="M2" s="32">
         <v>180</v>
       </c>
-      <c r="N2" s="33">
+      <c r="N2" s="32">
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -883,25 +879,47 @@
       <c r="C3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="Q3" s="31"/>
-      <c r="R3" s="31"/>
-      <c r="S3" s="31"/>
-      <c r="T3" s="31"/>
-      <c r="U3" s="31"/>
-      <c r="V3" s="31"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D3" s="5">
+        <v>100</v>
+      </c>
+      <c r="E3" s="5">
+        <v>100</v>
+      </c>
+      <c r="F3" s="5">
+        <v>100</v>
+      </c>
+      <c r="G3" s="5">
+        <v>100</v>
+      </c>
+      <c r="H3" s="5">
+        <v>100</v>
+      </c>
+      <c r="I3" s="5">
+        <v>100</v>
+      </c>
+      <c r="J3" s="5">
+        <v>100</v>
+      </c>
+      <c r="K3" s="5">
+        <v>100</v>
+      </c>
+      <c r="L3" s="5">
+        <v>100</v>
+      </c>
+      <c r="M3" s="5">
+        <v>100</v>
+      </c>
+      <c r="N3" s="5">
+        <v>100</v>
+      </c>
+      <c r="Q3" s="30"/>
+      <c r="R3" s="30"/>
+      <c r="S3" s="30"/>
+      <c r="T3" s="30"/>
+      <c r="U3" s="30"/>
+      <c r="V3" s="30"/>
+    </row>
+    <row r="4" spans="1:22">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -912,50 +930,50 @@
         <v>18</v>
       </c>
       <c r="D4" s="5">
-        <v>3843</v>
+        <v>1496</v>
       </c>
       <c r="E4" s="5">
-        <v>3057</v>
+        <v>1190</v>
       </c>
       <c r="F4" s="5">
-        <v>3232</v>
+        <v>1258</v>
       </c>
       <c r="G4" s="5">
-        <v>17468</v>
+        <v>6800</v>
       </c>
       <c r="H4" s="5">
-        <v>27600</v>
+        <v>3740</v>
       </c>
       <c r="I4" s="5">
-        <v>6289</v>
+        <v>2448</v>
       </c>
       <c r="J4" s="5">
-        <v>11616</v>
+        <v>4522</v>
       </c>
       <c r="K4" s="5">
-        <v>9171</v>
+        <v>3570</v>
       </c>
       <c r="L4" s="5">
-        <v>8734</v>
+        <v>3400</v>
       </c>
       <c r="M4" s="5">
-        <v>35810</v>
+        <v>6120</v>
       </c>
       <c r="N4" s="5">
-        <v>6813</v>
+        <v>2652</v>
       </c>
       <c r="O4">
         <f>SUM(D4:N4)</f>
-        <v>133633</v>
-      </c>
-      <c r="Q4" s="31"/>
-      <c r="R4" s="31"/>
-      <c r="S4" s="31"/>
-      <c r="T4" s="31"/>
-      <c r="U4" s="31"/>
-      <c r="V4" s="31"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+        <v>37196</v>
+      </c>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="30"/>
+      <c r="S4" s="30"/>
+      <c r="T4" s="30"/>
+      <c r="U4" s="30"/>
+      <c r="V4" s="30"/>
+    </row>
+    <row r="5" spans="1:22">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
@@ -966,50 +984,50 @@
         <v>19</v>
       </c>
       <c r="D5" s="5">
-        <v>1408</v>
+        <v>3603</v>
       </c>
       <c r="E5" s="5">
-        <v>1120</v>
+        <v>2866</v>
       </c>
       <c r="F5" s="5">
-        <v>1184</v>
+        <v>3030</v>
       </c>
       <c r="G5" s="5">
-        <v>6400</v>
+        <v>16376</v>
       </c>
       <c r="H5" s="5">
-        <v>3520</v>
+        <v>9007</v>
       </c>
       <c r="I5" s="5">
-        <v>2304</v>
+        <v>5896</v>
       </c>
       <c r="J5" s="5">
-        <v>4256</v>
+        <v>10890</v>
       </c>
       <c r="K5" s="5">
-        <v>3360</v>
+        <v>8598</v>
       </c>
       <c r="L5" s="5">
-        <v>3200</v>
+        <v>8188</v>
       </c>
       <c r="M5" s="5">
-        <v>5760</v>
+        <v>14739</v>
       </c>
       <c r="N5" s="5">
-        <v>2496</v>
+        <v>6387</v>
       </c>
       <c r="O5">
         <f>SUM(D5:N5)</f>
-        <v>35008</v>
-      </c>
-      <c r="Q5" s="31"/>
-      <c r="R5" s="31"/>
-      <c r="S5" s="31"/>
-      <c r="T5" s="31"/>
-      <c r="U5" s="31"/>
-      <c r="V5" s="31"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+        <v>89580</v>
+      </c>
+      <c r="Q5" s="30"/>
+      <c r="R5" s="30"/>
+      <c r="S5" s="30"/>
+      <c r="T5" s="30"/>
+      <c r="U5" s="30"/>
+      <c r="V5" s="30"/>
+    </row>
+    <row r="6" spans="1:22">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
@@ -1019,25 +1037,47 @@
       <c r="C6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="Q6" s="31"/>
-      <c r="R6" s="31"/>
-      <c r="S6" s="31"/>
-      <c r="T6" s="31"/>
-      <c r="U6" s="31"/>
-      <c r="V6" s="31"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D6" s="5">
+        <v>100</v>
+      </c>
+      <c r="E6" s="5">
+        <v>100</v>
+      </c>
+      <c r="F6" s="5">
+        <v>100</v>
+      </c>
+      <c r="G6" s="5">
+        <v>100</v>
+      </c>
+      <c r="H6" s="5">
+        <v>100</v>
+      </c>
+      <c r="I6" s="5">
+        <v>100</v>
+      </c>
+      <c r="J6" s="5">
+        <v>100</v>
+      </c>
+      <c r="K6" s="5">
+        <v>100</v>
+      </c>
+      <c r="L6" s="5">
+        <v>100</v>
+      </c>
+      <c r="M6" s="5">
+        <v>100</v>
+      </c>
+      <c r="N6" s="5">
+        <v>100</v>
+      </c>
+      <c r="Q6" s="30"/>
+      <c r="R6" s="30"/>
+      <c r="S6" s="30"/>
+      <c r="T6" s="30"/>
+      <c r="U6" s="30"/>
+      <c r="V6" s="30"/>
+    </row>
+    <row r="7" spans="1:22">
       <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
@@ -1080,14 +1120,14 @@
       <c r="N7" s="5">
         <v>1030</v>
       </c>
-      <c r="Q7" s="31"/>
-      <c r="R7" s="31"/>
-      <c r="S7" s="31"/>
-      <c r="T7" s="31"/>
-      <c r="U7" s="31"/>
-      <c r="V7" s="31"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Q7" s="30"/>
+      <c r="R7" s="30"/>
+      <c r="S7" s="30"/>
+      <c r="T7" s="30"/>
+      <c r="U7" s="30"/>
+      <c r="V7" s="30"/>
+    </row>
+    <row r="8" spans="1:22">
       <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
@@ -1130,14 +1170,14 @@
       <c r="N8" s="5">
         <v>108</v>
       </c>
-      <c r="Q8" s="31"/>
-      <c r="R8" s="31"/>
-      <c r="S8" s="31"/>
-      <c r="T8" s="31"/>
-      <c r="U8" s="31"/>
-      <c r="V8" s="31"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Q8" s="30"/>
+      <c r="R8" s="30"/>
+      <c r="S8" s="30"/>
+      <c r="T8" s="30"/>
+      <c r="U8" s="30"/>
+      <c r="V8" s="30"/>
+    </row>
+    <row r="9" spans="1:22">
       <c r="A9" s="5" t="s">
         <v>6</v>
       </c>
@@ -1180,14 +1220,14 @@
       <c r="N9" s="5">
         <v>1217</v>
       </c>
-      <c r="Q9" s="31"/>
-      <c r="R9" s="31"/>
-      <c r="S9" s="31"/>
-      <c r="T9" s="31"/>
-      <c r="U9" s="31"/>
-      <c r="V9" s="31"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Q9" s="30"/>
+      <c r="R9" s="30"/>
+      <c r="S9" s="30"/>
+      <c r="T9" s="30"/>
+      <c r="U9" s="30"/>
+      <c r="V9" s="30"/>
+    </row>
+    <row r="10" spans="1:22">
       <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
@@ -1230,14 +1270,14 @@
       <c r="N10" s="5">
         <v>122</v>
       </c>
-      <c r="Q10" s="31"/>
-      <c r="R10" s="31"/>
-      <c r="S10" s="31"/>
-      <c r="T10" s="31"/>
-      <c r="U10" s="31"/>
-      <c r="V10" s="31"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Q10" s="30"/>
+      <c r="R10" s="30"/>
+      <c r="S10" s="30"/>
+      <c r="T10" s="30"/>
+      <c r="U10" s="30"/>
+      <c r="V10" s="30"/>
+    </row>
+    <row r="11" spans="1:22">
       <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
@@ -1248,46 +1288,46 @@
         <v>25</v>
       </c>
       <c r="D11" s="5">
-        <v>5251</v>
+        <v>5099</v>
       </c>
       <c r="E11" s="5">
-        <v>4177</v>
+        <v>4056</v>
       </c>
       <c r="F11" s="5">
-        <v>4416</v>
+        <v>4288</v>
       </c>
       <c r="G11" s="5">
-        <v>23868</v>
+        <v>23176</v>
       </c>
       <c r="H11" s="5">
-        <v>31120</v>
+        <v>12747</v>
       </c>
       <c r="I11" s="5">
-        <v>8593</v>
+        <v>8344</v>
       </c>
       <c r="J11" s="5">
-        <v>15872</v>
+        <v>15412</v>
       </c>
       <c r="K11" s="5">
-        <v>12531</v>
+        <v>12168</v>
       </c>
       <c r="L11" s="5">
-        <v>11934</v>
+        <v>11588</v>
       </c>
       <c r="M11" s="5">
-        <v>41570</v>
+        <v>20859</v>
       </c>
       <c r="N11" s="5">
-        <v>9309</v>
-      </c>
-      <c r="Q11" s="31"/>
-      <c r="R11" s="31"/>
-      <c r="S11" s="31"/>
-      <c r="T11" s="31"/>
-      <c r="U11" s="31"/>
-      <c r="V11" s="31"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+        <v>9039</v>
+      </c>
+      <c r="Q11" s="30"/>
+      <c r="R11" s="30"/>
+      <c r="S11" s="30"/>
+      <c r="T11" s="30"/>
+      <c r="U11" s="30"/>
+      <c r="V11" s="30"/>
+    </row>
+    <row r="12" spans="1:22">
       <c r="A12" s="5" t="s">
         <v>9</v>
       </c>
@@ -1297,145 +1337,167 @@
       <c r="C12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="Q12" s="31"/>
-      <c r="R12" s="31"/>
-      <c r="S12" s="31"/>
-      <c r="T12" s="31"/>
-      <c r="U12" s="31"/>
-      <c r="V12" s="31"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="Q13" s="31"/>
-      <c r="R13" s="31"/>
-      <c r="S13" s="31"/>
-      <c r="T13" s="31"/>
-      <c r="U13" s="31"/>
-      <c r="V13" s="31"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D12" s="5">
+        <v>100</v>
+      </c>
+      <c r="E12" s="5">
+        <v>100</v>
+      </c>
+      <c r="F12" s="5">
+        <v>100</v>
+      </c>
+      <c r="G12" s="5">
+        <v>100</v>
+      </c>
+      <c r="H12" s="5">
+        <v>100</v>
+      </c>
+      <c r="I12" s="5">
+        <v>100</v>
+      </c>
+      <c r="J12" s="5">
+        <v>100</v>
+      </c>
+      <c r="K12" s="5">
+        <v>100</v>
+      </c>
+      <c r="L12" s="5">
+        <v>100</v>
+      </c>
+      <c r="M12" s="5">
+        <v>100</v>
+      </c>
+      <c r="N12" s="5">
+        <v>100</v>
+      </c>
+      <c r="Q12" s="30"/>
+      <c r="R12" s="30"/>
+      <c r="S12" s="30"/>
+      <c r="T12" s="30"/>
+      <c r="U12" s="30"/>
+      <c r="V12" s="30"/>
+    </row>
+    <row r="13" spans="1:22">
+      <c r="Q13" s="30"/>
+      <c r="R13" s="30"/>
+      <c r="S13" s="30"/>
+      <c r="T13" s="30"/>
+      <c r="U13" s="30"/>
+      <c r="V13" s="30"/>
+    </row>
+    <row r="14" spans="1:22">
       <c r="D14" s="3">
-        <f>SUM(D4:D5)</f>
-        <v>5251</v>
+        <f>34*D2</f>
+        <v>1496</v>
       </c>
       <c r="E14" s="3">
-        <f t="shared" ref="E14:N14" si="0">SUM(E4:E5)</f>
-        <v>4177</v>
+        <f t="shared" ref="E14:N14" si="0">34*E2</f>
+        <v>1190</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" si="0"/>
-        <v>4416</v>
+        <v>1258</v>
       </c>
       <c r="G14" s="3">
         <f t="shared" si="0"/>
-        <v>23868</v>
+        <v>6800</v>
       </c>
       <c r="H14" s="3">
         <f t="shared" si="0"/>
-        <v>31120</v>
+        <v>3740</v>
       </c>
       <c r="I14" s="3">
         <f t="shared" si="0"/>
-        <v>8593</v>
+        <v>2448</v>
       </c>
       <c r="J14" s="3">
         <f t="shared" si="0"/>
-        <v>15872</v>
+        <v>4522</v>
       </c>
       <c r="K14" s="3">
         <f t="shared" si="0"/>
-        <v>12531</v>
+        <v>3570</v>
       </c>
       <c r="L14" s="3">
         <f t="shared" si="0"/>
-        <v>11934</v>
+        <v>3400</v>
       </c>
       <c r="M14" s="3">
         <f t="shared" si="0"/>
-        <v>41570</v>
+        <v>6120</v>
       </c>
       <c r="N14" s="3">
         <f t="shared" si="0"/>
-        <v>9309</v>
+        <v>2652</v>
       </c>
       <c r="O14" s="3">
         <f>SUM(D14:N14)</f>
-        <v>168641</v>
-      </c>
-      <c r="Q14" s="32"/>
-      <c r="R14" s="32"/>
-      <c r="S14" s="32"/>
-      <c r="T14" s="32"/>
-      <c r="U14" s="32"/>
-      <c r="V14" s="32"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+        <v>37196</v>
+      </c>
+      <c r="Q14" s="31"/>
+      <c r="R14" s="31"/>
+      <c r="S14" s="31"/>
+      <c r="T14" s="31"/>
+      <c r="U14" s="31"/>
+      <c r="V14" s="31"/>
+    </row>
+    <row r="15" spans="1:22">
       <c r="D15" s="3">
         <f>_xlfn.CEILING.MATH(D14,1)</f>
-        <v>5251</v>
+        <v>1496</v>
       </c>
       <c r="E15" s="3">
         <f t="shared" ref="E15:N15" si="1">_xlfn.CEILING.MATH(E14,1)</f>
-        <v>4177</v>
+        <v>1190</v>
       </c>
       <c r="F15" s="3">
         <f t="shared" si="1"/>
-        <v>4416</v>
+        <v>1258</v>
       </c>
       <c r="G15" s="3">
         <f t="shared" si="1"/>
-        <v>23868</v>
+        <v>6800</v>
       </c>
       <c r="H15" s="3">
         <f t="shared" si="1"/>
-        <v>31120</v>
+        <v>3740</v>
       </c>
       <c r="I15" s="3">
         <f t="shared" si="1"/>
-        <v>8593</v>
+        <v>2448</v>
       </c>
       <c r="J15" s="3">
         <f t="shared" si="1"/>
-        <v>15872</v>
+        <v>4522</v>
       </c>
       <c r="K15" s="3">
         <f t="shared" si="1"/>
-        <v>12531</v>
+        <v>3570</v>
       </c>
       <c r="L15" s="3">
         <f t="shared" si="1"/>
-        <v>11934</v>
+        <v>3400</v>
       </c>
       <c r="M15" s="3">
         <f t="shared" si="1"/>
-        <v>41570</v>
+        <v>6120</v>
       </c>
       <c r="N15" s="3">
         <f t="shared" si="1"/>
-        <v>9309</v>
+        <v>2652</v>
       </c>
       <c r="O15" s="3">
         <f>SUM(D15:N15)</f>
-        <v>168641</v>
-      </c>
-      <c r="Q15" s="32"/>
-      <c r="R15" s="32"/>
-      <c r="S15" s="32"/>
-      <c r="T15" s="32"/>
-      <c r="U15" s="32"/>
-      <c r="V15" s="32"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+        <v>37196</v>
+      </c>
+      <c r="Q15" s="31"/>
+      <c r="R15" s="31"/>
+      <c r="S15" s="31"/>
+      <c r="T15" s="31"/>
+      <c r="U15" s="31"/>
+      <c r="V15" s="31"/>
+    </row>
+    <row r="16" spans="1:22">
       <c r="A16" s="3" t="s">
         <v>53</v>
       </c>
@@ -1452,7 +1514,7 @@
       <c r="S16" s="13"/>
       <c r="T16" s="14"/>
     </row>
-    <row r="17" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" ht="28.8">
       <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
@@ -1462,20 +1524,20 @@
       <c r="C17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="30" t="s">
+      <c r="D17" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="30" t="s">
+      <c r="F17" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="F17" s="30" t="s">
+      <c r="G17" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="G17" s="30" t="s">
+      <c r="H17" s="29" t="s">
         <v>73</v>
-      </c>
-      <c r="H17" s="30" t="s">
-        <v>74</v>
       </c>
       <c r="I17" s="11"/>
       <c r="J17" s="13"/>
@@ -1489,9 +1551,9 @@
       <c r="R17" s="12"/>
       <c r="S17" s="13"/>
       <c r="T17" s="14"/>
-      <c r="U17" s="32"/>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U17" s="31"/>
+    </row>
+    <row r="18" spans="1:21">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1517,14 +1579,14 @@
       <c r="M18" s="13"/>
       <c r="N18" s="13"/>
       <c r="O18" s="13"/>
-      <c r="P18" s="27"/>
-      <c r="Q18" s="26"/>
-      <c r="R18" s="27"/>
-      <c r="S18" s="26"/>
-      <c r="T18" s="27"/>
-      <c r="U18" s="28"/>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="P18" s="26"/>
+      <c r="Q18" s="25"/>
+      <c r="R18" s="26"/>
+      <c r="S18" s="25"/>
+      <c r="T18" s="26"/>
+      <c r="U18" s="27"/>
+    </row>
+    <row r="19" spans="1:21">
       <c r="A19" s="2" t="s">
         <v>27</v>
       </c>
@@ -1534,11 +1596,21 @@
       <c r="C19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
+      <c r="D19" s="2">
+        <v>100</v>
+      </c>
+      <c r="E19" s="2">
+        <v>100</v>
+      </c>
+      <c r="F19" s="2">
+        <v>100</v>
+      </c>
+      <c r="G19" s="2">
+        <v>100</v>
+      </c>
+      <c r="H19" s="2">
+        <v>100</v>
+      </c>
       <c r="I19" s="13"/>
       <c r="J19" s="13"/>
       <c r="K19" s="13"/>
@@ -1546,14 +1618,14 @@
       <c r="M19" s="13"/>
       <c r="N19" s="13"/>
       <c r="O19" s="13"/>
-      <c r="P19" s="27"/>
-      <c r="Q19" s="26"/>
-      <c r="R19" s="27"/>
-      <c r="S19" s="26"/>
-      <c r="T19" s="27"/>
-      <c r="U19" s="28"/>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="P19" s="26"/>
+      <c r="Q19" s="25"/>
+      <c r="R19" s="26"/>
+      <c r="S19" s="25"/>
+      <c r="T19" s="26"/>
+      <c r="U19" s="27"/>
+    </row>
+    <row r="20" spans="1:21">
       <c r="A20" s="1" t="s">
         <v>28</v>
       </c>
@@ -1579,22 +1651,22 @@
         <v>2187</v>
       </c>
       <c r="I20" s="13"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="24"/>
-      <c r="N20" s="24"/>
-      <c r="O20" s="24"/>
-      <c r="P20" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q20" s="26"/>
-      <c r="R20" s="27"/>
-      <c r="S20" s="26"/>
-      <c r="T20" s="27"/>
-      <c r="U20" s="28"/>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="23"/>
+      <c r="P20" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q20" s="25"/>
+      <c r="R20" s="26"/>
+      <c r="S20" s="25"/>
+      <c r="T20" s="26"/>
+      <c r="U20" s="27"/>
+    </row>
+    <row r="21" spans="1:21">
       <c r="A21" s="1" t="s">
         <v>29</v>
       </c>
@@ -1619,23 +1691,23 @@
       <c r="H21" s="5">
         <v>2429</v>
       </c>
-      <c r="I21" s="16"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="34"/>
-      <c r="L21" s="34"/>
-      <c r="M21" s="34"/>
-      <c r="N21" s="34"/>
-      <c r="O21" s="34"/>
-      <c r="P21" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q21" s="31"/>
-      <c r="R21" s="31"/>
-      <c r="S21" s="31"/>
-      <c r="T21" s="31"/>
-      <c r="U21" s="32"/>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="I21" s="15"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="33"/>
+      <c r="M21" s="33"/>
+      <c r="N21" s="33"/>
+      <c r="O21" s="33"/>
+      <c r="P21" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q21" s="30"/>
+      <c r="R21" s="30"/>
+      <c r="S21" s="30"/>
+      <c r="T21" s="30"/>
+      <c r="U21" s="31"/>
+    </row>
+    <row r="22" spans="1:21">
       <c r="A22" s="1" t="s">
         <v>65</v>
       </c>
@@ -1643,714 +1715,740 @@
         <v>13</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="D22" s="5">
-        <v>1700</v>
+        <v>5861</v>
       </c>
       <c r="E22" s="5">
-        <v>668</v>
+        <v>2303</v>
       </c>
       <c r="F22" s="5">
-        <v>400</v>
+        <v>1379</v>
       </c>
       <c r="G22" s="5">
-        <v>1020</v>
+        <v>3517</v>
       </c>
       <c r="H22" s="5">
-        <v>600</v>
-      </c>
-      <c r="I22" s="16"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="34"/>
-      <c r="L22" s="34"/>
-      <c r="M22" s="34"/>
-      <c r="N22" s="34"/>
-      <c r="O22" s="34"/>
-      <c r="P22" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q22" s="31"/>
-      <c r="R22" s="31"/>
-      <c r="S22" s="31"/>
-      <c r="T22" s="31"/>
-      <c r="U22" s="32"/>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+        <v>2069</v>
+      </c>
+      <c r="I22" s="15"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="33"/>
+      <c r="L22" s="33"/>
+      <c r="M22" s="33"/>
+      <c r="N22" s="33"/>
+      <c r="O22" s="33"/>
+      <c r="P22" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q22" s="30"/>
+      <c r="R22" s="30"/>
+      <c r="S22" s="30"/>
+      <c r="T22" s="30"/>
+      <c r="U22" s="31"/>
+    </row>
+    <row r="23" spans="1:21">
       <c r="A23" s="1" t="s">
-        <v>66</v>
+        <v>9</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="34"/>
-      <c r="K23" s="34"/>
-      <c r="L23" s="34"/>
-      <c r="M23" s="34"/>
-      <c r="N23" s="34"/>
-      <c r="O23" s="34"/>
-      <c r="P23" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q23" s="31"/>
-      <c r="R23" s="31"/>
-      <c r="S23" s="31"/>
-      <c r="T23" s="31"/>
-      <c r="U23" s="32"/>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="24"/>
-      <c r="L24" s="24"/>
-      <c r="M24" s="24"/>
-      <c r="N24" s="24"/>
-      <c r="O24" s="24"/>
-      <c r="P24" s="23"/>
-      <c r="Q24" s="24"/>
-      <c r="R24" s="23"/>
-      <c r="S24" s="24"/>
-      <c r="T24" s="25"/>
-      <c r="U24" s="32"/>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="I25" s="22"/>
-      <c r="J25" s="24"/>
-      <c r="K25" s="24"/>
-      <c r="L25" s="24"/>
-      <c r="M25" s="24"/>
-      <c r="N25" s="24"/>
-      <c r="O25" s="24"/>
-      <c r="P25" s="23"/>
-      <c r="Q25" s="24"/>
-      <c r="R25" s="23"/>
-      <c r="S25" s="24"/>
-      <c r="T25" s="25"/>
-      <c r="U25" s="32"/>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D23" s="1">
+        <v>100</v>
+      </c>
+      <c r="E23" s="1">
+        <v>100</v>
+      </c>
+      <c r="F23" s="1">
+        <v>100</v>
+      </c>
+      <c r="G23" s="1">
+        <v>100</v>
+      </c>
+      <c r="H23" s="1">
+        <v>100</v>
+      </c>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="23"/>
+      <c r="O23" s="23"/>
+      <c r="P23" s="22"/>
+      <c r="Q23" s="23"/>
+      <c r="R23" s="22"/>
+      <c r="S23" s="23"/>
+      <c r="T23" s="24"/>
+      <c r="U23" s="31"/>
+    </row>
+    <row r="24" spans="1:21">
+      <c r="I24" s="21"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="22"/>
+      <c r="Q24" s="23"/>
+      <c r="R24" s="22"/>
+      <c r="S24" s="23"/>
+      <c r="T24" s="24"/>
+      <c r="U24" s="31"/>
+    </row>
+    <row r="25" spans="1:21">
+      <c r="D25">
+        <f>13.79*D18</f>
+        <v>5860.75</v>
+      </c>
+      <c r="E25">
+        <f t="shared" ref="E25:H25" si="2">13.79*E18</f>
+        <v>2302.9299999999998</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="2"/>
+        <v>1379</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="2"/>
+        <v>3516.45</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="2"/>
+        <v>2068.5</v>
+      </c>
+      <c r="I25" s="21"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="23"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="23"/>
+      <c r="O25" s="23"/>
+      <c r="P25" s="22"/>
+      <c r="Q25" s="23"/>
+      <c r="R25" s="22"/>
+      <c r="S25" s="23"/>
+      <c r="T25" s="24"/>
+      <c r="U25" s="31"/>
+    </row>
+    <row r="26" spans="1:21">
       <c r="D26">
-        <f>4*D18</f>
-        <v>1700</v>
+        <f>_xlfn.CEILING.MATH(D25,1)</f>
+        <v>5861</v>
       </c>
       <c r="E26">
-        <f t="shared" ref="E26:H26" si="2">4*E18</f>
-        <v>668</v>
+        <f t="shared" ref="E26:H26" si="3">_xlfn.CEILING.MATH(E25,1)</f>
+        <v>2303</v>
       </c>
       <c r="F26">
-        <f t="shared" si="2"/>
-        <v>400</v>
+        <f t="shared" si="3"/>
+        <v>1379</v>
       </c>
       <c r="G26">
-        <f t="shared" si="2"/>
-        <v>1020</v>
+        <f t="shared" si="3"/>
+        <v>3517</v>
       </c>
       <c r="H26">
-        <f t="shared" si="2"/>
-        <v>600</v>
-      </c>
-      <c r="I26" s="22"/>
-      <c r="J26" s="24"/>
-      <c r="K26" s="24"/>
-      <c r="L26" s="24"/>
-      <c r="M26" s="24"/>
-      <c r="N26" s="24"/>
-      <c r="O26" s="24"/>
-      <c r="P26" s="23"/>
-      <c r="Q26" s="24"/>
-      <c r="R26" s="23"/>
-      <c r="S26" s="24"/>
-      <c r="T26" s="25"/>
-      <c r="U26" s="32"/>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D27">
-        <f>_xlfn.CEILING.MATH(D26,1)</f>
-        <v>1700</v>
-      </c>
-      <c r="E27">
-        <f t="shared" ref="E27:H27" si="3">_xlfn.CEILING.MATH(E26,1)</f>
-        <v>668</v>
-      </c>
-      <c r="F27">
         <f t="shared" si="3"/>
-        <v>400</v>
-      </c>
-      <c r="G27">
-        <f t="shared" si="3"/>
-        <v>1020</v>
-      </c>
-      <c r="H27">
-        <f t="shared" si="3"/>
-        <v>600</v>
-      </c>
-      <c r="I27" s="17">
-        <f>SUM(D27:H27)</f>
-        <v>4388</v>
-      </c>
-      <c r="J27" s="29"/>
-      <c r="K27" s="29"/>
-      <c r="L27" s="29"/>
-      <c r="M27" s="29"/>
-      <c r="N27" s="29"/>
-      <c r="O27" s="29"/>
-      <c r="P27" s="18"/>
-      <c r="Q27" s="19"/>
-      <c r="R27" s="20"/>
-      <c r="S27" s="19"/>
-      <c r="T27" s="21"/>
-      <c r="U27" s="32"/>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+        <v>2069</v>
+      </c>
+      <c r="I26" s="16">
+        <f>SUM(D26:H26)</f>
+        <v>15129</v>
+      </c>
+      <c r="J26" s="28"/>
+      <c r="K26" s="28"/>
+      <c r="L26" s="28"/>
+      <c r="M26" s="28"/>
+      <c r="N26" s="28"/>
+      <c r="O26" s="28"/>
+      <c r="P26" s="17"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="18"/>
+      <c r="T26" s="20"/>
+      <c r="U26" s="31"/>
+    </row>
+    <row r="27" spans="1:21">
+      <c r="A27" t="s">
+        <v>75</v>
+      </c>
+      <c r="F27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21">
+      <c r="A28" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L28">
+        <v>5610</v>
+      </c>
+      <c r="M28">
+        <v>2205</v>
+      </c>
+      <c r="N28">
+        <v>1320</v>
+      </c>
+      <c r="O28">
+        <v>3366</v>
+      </c>
+      <c r="P28">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21">
       <c r="A29" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>51</v>
+        <v>30</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="1">
+        <v>100</v>
       </c>
       <c r="L29">
-        <v>5610</v>
+        <v>587</v>
       </c>
       <c r="M29">
-        <v>2205</v>
+        <v>231</v>
       </c>
       <c r="N29">
-        <v>1320</v>
+        <v>138</v>
       </c>
       <c r="O29">
-        <v>3366</v>
+        <v>352</v>
       </c>
       <c r="P29">
-        <v>1980</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>30</v>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21">
+      <c r="A30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" s="15"/>
+        <v>45</v>
+      </c>
+      <c r="D30" s="5">
+        <v>1798</v>
+      </c>
       <c r="L30">
-        <v>587</v>
+        <f>SUM(L28:L29)</f>
+        <v>6197</v>
       </c>
       <c r="M30">
-        <v>231</v>
+        <f t="shared" ref="M30:P30" si="4">SUM(M28:M29)</f>
+        <v>2436</v>
       </c>
       <c r="N30">
-        <v>138</v>
+        <f t="shared" si="4"/>
+        <v>1458</v>
       </c>
       <c r="O30">
-        <v>352</v>
+        <f t="shared" si="4"/>
+        <v>3718</v>
       </c>
       <c r="P30">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>2187</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21">
       <c r="A31" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D31" s="5">
-        <v>1798</v>
-      </c>
-      <c r="L31">
-        <f>SUM(L29:L30)</f>
-        <v>6197</v>
-      </c>
-      <c r="M31">
-        <f t="shared" ref="M31:P31" si="4">SUM(M29:M30)</f>
-        <v>2436</v>
-      </c>
-      <c r="N31">
-        <f t="shared" si="4"/>
-        <v>1458</v>
-      </c>
-      <c r="O31">
-        <f t="shared" si="4"/>
-        <v>3718</v>
-      </c>
-      <c r="P31">
-        <f t="shared" si="4"/>
-        <v>2187</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+        <v>7312</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21">
       <c r="A32" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D32" s="5">
-        <v>7312</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1781</v>
+      </c>
+      <c r="F32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C33" s="10" t="s">
-        <v>47</v>
+      <c r="C33" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="D33" s="5">
-        <v>1781</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+        <v>3917</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D34" s="5">
-        <v>3917</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D35" s="15"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="D35" s="5">
+        <v>2052</v>
+      </c>
+      <c r="H35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D36" s="5">
-        <v>2052</v>
-      </c>
-      <c r="H36" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1598</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="D37" s="5">
-        <v>1598</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+        <v>4479</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="10" t="s">
-        <v>21</v>
+      <c r="C38" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="D38" s="5">
-        <v>4479</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D39" s="5">
+        <v>3117</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C39" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D39" s="5">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="C40" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D40" s="5">
-        <v>3117</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D41" s="5">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="D41" s="34">
+        <v>4047</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D42" s="35">
-        <v>4047</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="D42" s="5">
+        <v>14808</v>
+      </c>
+      <c r="F42" s="3"/>
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D43" s="5">
+        <v>1641</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D44" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D51" s="2"/>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B52" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C43" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D43" s="5">
-        <v>14808</v>
-      </c>
-      <c r="F43" s="3"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D44" s="5">
-        <v>1641</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C45" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D45" s="15"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="C52" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D52" s="2"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="D52" s="5">
+        <v>2841</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D53" s="5">
-        <v>2841</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5557</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D54" s="5">
-        <v>5557</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3563</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="D55" s="5">
-        <v>3563</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3875</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D56" s="5">
-        <v>3875</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="D56" s="2"/>
+    </row>
+    <row r="57" spans="1:4">
       <c r="A57" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D57" s="2"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="D57" s="5">
+        <v>2052</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D58" s="5">
-        <v>2052</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59" s="4" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="D59" s="5">
-        <v>2665</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2837</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60" s="4" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D60" s="5">
-        <v>2837</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
       <c r="A61" s="4" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B61" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D61" s="5">
+        <v>2915</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B62" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C61" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D61" s="5">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="C62" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D62" s="5">
-        <v>2915</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
       <c r="A63" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D63" s="5">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3071</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
       <c r="A64" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D64" s="5">
-        <v>3071</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="D64" s="34">
+        <v>15836</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15">
       <c r="A65" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D65" s="35">
-        <v>15836</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="D65" s="5">
+        <v>1641</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15">
       <c r="A66" s="4" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D66" s="5">
-        <v>1641</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C67" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D67" s="2"/>
+      <c r="D66" s="2"/>
+    </row>
+    <row r="71" spans="1:15">
+      <c r="E71">
+        <v>3603</v>
+      </c>
+      <c r="F71">
+        <v>2866</v>
+      </c>
+      <c r="G71">
+        <v>3030</v>
+      </c>
+      <c r="H71">
+        <v>16376</v>
+      </c>
+      <c r="I71">
+        <v>9007</v>
+      </c>
+      <c r="J71">
+        <v>5896</v>
+      </c>
+      <c r="K71">
+        <v>10890</v>
+      </c>
+      <c r="L71">
+        <v>8598</v>
+      </c>
+      <c r="M71">
+        <v>8188</v>
+      </c>
+      <c r="N71">
+        <v>14739</v>
+      </c>
+      <c r="O71">
+        <v>6387</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>